<commit_message>
Added PJRC stuff to BOM
</commit_message>
<xml_diff>
--- a/Version 2 (Latest)/Hardware/Bill of Materials/V2.3BOM.xlsx
+++ b/Version 2 (Latest)/Hardware/Bill of Materials/V2.3BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Portfolio Things\Synth V2\2.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54258D3E-DE98-4B7C-BEB2-4F1EB3A1D297}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC27F78C-FC74-4770-8E0C-3EC00435000B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17775" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DIGIKEY BOM" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="237">
   <si>
     <t>Manufacturer Part Number</t>
   </si>
@@ -718,6 +718,21 @@
   </si>
   <si>
     <t>CART LINK: https://www.digikey.com/short/4734rh</t>
+  </si>
+  <si>
+    <t>PJRC</t>
+  </si>
+  <si>
+    <t>Teensy 4.1</t>
+  </si>
+  <si>
+    <t>http://bit.ly/3ibYI2y</t>
+  </si>
+  <si>
+    <t>PSRAM Chip</t>
+  </si>
+  <si>
+    <t>http://bit.ly/3nQR6nC</t>
   </si>
 </sst>
 </file>
@@ -1669,8 +1684,8 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3006,10 +3021,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3021,7 +3036,7 @@
     <col min="5" max="5" width="23.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="13" t="s">
         <v>227</v>
       </c>
@@ -3030,7 +3045,7 @@
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>220</v>
       </c>
@@ -3047,7 +3062,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>225</v>
       </c>
@@ -3064,21 +3079,21 @@
         <v>226</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A6" s="13" t="s">
         <v>228</v>
       </c>
@@ -3087,7 +3102,7 @@
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>220</v>
       </c>
@@ -3104,7 +3119,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>229</v>
       </c>
@@ -3121,23 +3136,89 @@
         <v>230</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
+    <row r="11" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A11" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" s="11">
+        <v>26.85</v>
+      </c>
+      <c r="D13" s="11">
+        <v>26.85</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B14" s="2">
+        <v>2</v>
+      </c>
+      <c r="C14" s="11">
+        <v>1.2</v>
+      </c>
+      <c r="D14" s="11">
+        <v>2.4</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="F14" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A11:E11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
     <hyperlink ref="E8" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E13" r:id="rId3" xr:uid="{BDD10C30-9DD8-429B-A74A-74FF00E3A3F8}"/>
+    <hyperlink ref="E14" r:id="rId4" xr:uid="{F1080651-A34C-4F44-A0AC-A401A34DD68F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" r:id="rId3"/>
+  <pageSetup orientation="landscape" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>